<commit_message>
added unloaded palletized charge report
</commit_message>
<xml_diff>
--- a/InAcc.xlsx
+++ b/InAcc.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+  <si>
+    <t>APPT FEE</t>
+  </si>
+  <si>
+    <t>OverFlow:InboundPallets</t>
+  </si>
   <si>
     <t>UNLD 20 FT FLR CNT</t>
   </si>
@@ -25,6 +31,12 @@
     <t>UNLD 45 FT FLR CNT</t>
   </si>
   <si>
+    <t>Vehicle Inspection-Inbound</t>
+  </si>
+  <si>
+    <t>Appointment Fee</t>
+  </si>
+  <si>
     <t>Unload 20 ft floor loaded</t>
   </si>
   <si>
@@ -32,6 +44,9 @@
   </si>
   <si>
     <t>Unload 45 ft floor loaded</t>
+  </si>
+  <si>
+    <t>Missed or Uncheduled Delivery Appointment</t>
   </si>
   <si>
     <t>WarehouseReceiptView</t>
@@ -404,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,22 +459,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -470,21 +473,9 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -496,22 +487,85 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>